<commit_message>
Update: Fix cell export
</commit_message>
<xml_diff>
--- a/public/FPD.xlsx
+++ b/public/FPD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\MLP\Approval\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA01959-A55E-4973-8FFD-42249BE87415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE74A957-A0A3-49FA-B8E1-BCE39F127223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{DF3E6CFB-0944-46E3-B09C-5D498E7CCF0E}"/>
   </bookViews>
@@ -330,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -378,6 +378,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -386,27 +404,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1008,96 +1005,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="1.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="17.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
@@ -1141,153 +1138,153 @@
       <c r="A16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
     </row>
     <row r="27" spans="1:8" ht="5.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
@@ -1305,27 +1302,27 @@
       <c r="A30" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="15" t="s">
@@ -1355,73 +1352,73 @@
       <c r="A34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
     </row>
     <row r="36" spans="1:8" ht="28.3" x14ac:dyDescent="0.4">
       <c r="A36" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="7"/>
@@ -1435,27 +1432,27 @@
       <c r="A42" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
     </row>
     <row r="43" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="10"/>
@@ -1472,28 +1469,28 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="17" t="s">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17" t="s">
+      <c r="D48" s="23"/>
+      <c r="E48" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17" t="s">
+      <c r="F48" s="23"/>
+      <c r="G48" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="H48" s="17"/>
+      <c r="H48" s="23"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A50" s="8"/>
@@ -1501,11 +1498,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:H7"/>
-    <mergeCell ref="B16:H17"/>
-    <mergeCell ref="A8:H9"/>
-    <mergeCell ref="B18:H19"/>
-    <mergeCell ref="B20:H21"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="B34:H35"/>
     <mergeCell ref="B32:H33"/>
     <mergeCell ref="B36:H37"/>
@@ -1514,14 +1514,11 @@
     <mergeCell ref="B24:H25"/>
     <mergeCell ref="A26:H27"/>
     <mergeCell ref="B30:H31"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A1:H7"/>
+    <mergeCell ref="B16:H17"/>
+    <mergeCell ref="A8:H9"/>
+    <mergeCell ref="B18:H19"/>
+    <mergeCell ref="B20:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" scale="92" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>